<commit_message>
updated heatmaps; added new platemap
</commit_message>
<xml_diff>
--- a/annotation/error_annotation.xlsx
+++ b/annotation/error_annotation.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\Documents\HNSCC_functional_data_pipeline\annotation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathiech\AppData\Local\Box\Box Edit\Documents\zgd3+cwoJUOlF9kjItjgDg==\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB7BAA3-9691-4DD7-B1D3-37864A18FE66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13950" yWindow="-15255" windowWidth="17325" windowHeight="15045" xr2:uid="{75DB37E0-52CC-4D69-AF7A-273E2B7B8DC0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="54">
   <si>
     <t>plate_number</t>
   </si>
@@ -55,12 +54,150 @@
   </si>
   <si>
     <t>remove</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>may be affected, remove if divergent from other pts trends for this drug</t>
+  </si>
+  <si>
+    <t>lab_id=10348-norm=Blank490-plate_version_id=OHSU_HNSCC_derm002-note=NA</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>blank first column of plate 4</t>
+  </si>
+  <si>
+    <t>lab_id=10326-norm=Blank490-plate_version_id=OHSU_HNSCC_derm002-note=NA</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>lab_id=20003-norm=blank490-plate_version_id=OHSU_HNSCC_derm002-note=NA</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Uneven cell growth across plate, using plate averaged controls will give poor results</t>
+  </si>
+  <si>
+    <t>Watch. Possibly affected, may need to be removed</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Don’t use these two wells for PAC; the drugs to the left of these wells appear unaffected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">watch </t>
+  </si>
+  <si>
+    <t>multidrop not primed before MTS or cells on plate 1; col 1-4 are affected</t>
+  </si>
+  <si>
+    <t>col 1-3 affected</t>
+  </si>
+  <si>
+    <t>col 1-2 affected</t>
+  </si>
+  <si>
+    <t>col 4-16 affected</t>
+  </si>
+  <si>
+    <t>col 9-12 affected</t>
+  </si>
+  <si>
+    <t>col 17-18 may be affected, remove if divergent from other pts trends for this drug (not as bad as others)</t>
+  </si>
+  <si>
+    <t>col 1-2 may be affected, Watch. Possibly affected, may need to be removed</t>
+  </si>
+  <si>
+    <t>col 1 may be affected,Watch. Possibly affected, may need to be removed</t>
+  </si>
+  <si>
+    <t>col 2 may be affected</t>
+  </si>
+  <si>
+    <t>col 1 may be affected, blank column 1</t>
+  </si>
+  <si>
+    <t>col 9-12 possibly affected</t>
+  </si>
+  <si>
+    <t>col 1-3 possibly affected</t>
+  </si>
+  <si>
+    <t>lab_id=10021-norm=Blank490-plate_version_id=OHSU_HNSCC_derm003-note=NA</t>
+  </si>
+  <si>
+    <t>lab_id=10054-norm=Blank490-plate_version_id=OHSU_HNSCC_derm003-note=NA</t>
+  </si>
+  <si>
+    <t>lab_id=10058-norm=Blank490-plate_version_id=OHSU_HNSCC_derm003-note=NA</t>
+  </si>
+  <si>
+    <t>lab_id=10139-norm=Blank490-plate_version_id=OHSU_HNSCC_derm003-note=NA</t>
+  </si>
+  <si>
+    <t>lab_id=10159-norm=Blank490-plate_version_id=OHSU_HNSCC_derm003-note=NA</t>
+  </si>
+  <si>
+    <t>lab_id=10205-norm=Blank490-plate_version_id=OHSU_HNSCC_derm003-note=NA</t>
+  </si>
+  <si>
+    <t>lab_id=10250-norm=Blank490-plate_version_id=OHSU_HNSCC_derm003-note=NA</t>
+  </si>
+  <si>
+    <t>lab_id=10289-norm=Blank490-plate_version_id=OHSU_HNSCC_derm003-note=NA</t>
+  </si>
+  <si>
+    <t>lab_id=10290-norm=Blank490-plate_version_id=OHSU_HNSCC_derm003-note=NA</t>
+  </si>
+  <si>
+    <t>lab_id=10292-norm=Blank490-plate_version_id=OHSU_HNSCC_derm003-note=NA</t>
+  </si>
+  <si>
+    <t>lab_id=10308-norm=Blank490-plate_version_id=OHSU_HNSCC_derm003-note=NA</t>
+  </si>
+  <si>
+    <t>lab_id=10356-norm=Blank490-plate_version_id=OHSU_HNSCC_derm002-note=NA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -90,8 +227,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,24 +545,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCA377FC-F97F-4F08-995F-C7F16C7609B8}">
-  <dimension ref="A1:H1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N44" sqref="N44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.1796875" customWidth="1"/>
-    <col min="2" max="2" width="17.36328125" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" customWidth="1"/>
-    <col min="7" max="7" width="61.81640625" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="61.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
@@ -440,14 +580,1351 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>9</v>
+      </c>
+      <c r="D9">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>16</v>
+      </c>
+      <c r="D10">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>17</v>
+      </c>
+      <c r="D11">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="D12">
+        <v>16</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>17</v>
+      </c>
+      <c r="D13">
+        <v>24</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>9</v>
+      </c>
+      <c r="D17">
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
+      </c>
+      <c r="E18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>9</v>
+      </c>
+      <c r="D19">
+        <v>16</v>
+      </c>
+      <c r="E19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>17</v>
+      </c>
+      <c r="D20">
+        <v>24</v>
+      </c>
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
+      <c r="E21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" t="s">
+        <v>27</v>
+      </c>
+      <c r="H21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>8</v>
+      </c>
+      <c r="E22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>8</v>
+      </c>
+      <c r="E23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <v>17</v>
+      </c>
+      <c r="D24">
+        <v>24</v>
+      </c>
+      <c r="E24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <v>9</v>
+      </c>
+      <c r="D25">
+        <v>16</v>
+      </c>
+      <c r="E25" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <v>9</v>
+      </c>
+      <c r="D26">
+        <v>16</v>
+      </c>
+      <c r="E26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27">
+        <v>5</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>8</v>
+      </c>
+      <c r="E27" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>8</v>
+      </c>
+      <c r="E28" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" t="s">
+        <v>24</v>
+      </c>
+      <c r="H28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>16</v>
+      </c>
+      <c r="E29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30">
+        <v>5</v>
+      </c>
+      <c r="C30">
+        <v>17</v>
+      </c>
+      <c r="D30">
+        <v>24</v>
+      </c>
+      <c r="E30" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <v>9</v>
+      </c>
+      <c r="D31">
+        <v>16</v>
+      </c>
+      <c r="E31" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32">
+        <v>5</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>16</v>
+      </c>
+      <c r="E32" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33">
+        <v>5</v>
+      </c>
+      <c r="C33">
+        <v>9</v>
+      </c>
+      <c r="D33">
+        <v>16</v>
+      </c>
+      <c r="E33" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34">
+        <v>17</v>
+      </c>
+      <c r="D34">
+        <v>24</v>
+      </c>
+      <c r="E34" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>8</v>
+      </c>
+      <c r="E35" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>8</v>
+      </c>
+      <c r="E36" t="s">
+        <v>16</v>
+      </c>
+      <c r="F36" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>8</v>
+      </c>
+      <c r="E37" t="s">
+        <v>17</v>
+      </c>
+      <c r="F37" t="s">
+        <v>17</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>8</v>
+      </c>
+      <c r="E38" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" t="s">
+        <v>18</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>8</v>
+      </c>
+      <c r="E39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" t="s">
+        <v>19</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>8</v>
+      </c>
+      <c r="E40" t="s">
+        <v>20</v>
+      </c>
+      <c r="F40" t="s">
+        <v>20</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>8</v>
+      </c>
+      <c r="E41" t="s">
+        <v>21</v>
+      </c>
+      <c r="F41" t="s">
+        <v>21</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>8</v>
+      </c>
+      <c r="E42" t="s">
+        <v>22</v>
+      </c>
+      <c r="F42" t="s">
+        <v>22</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43">
+        <v>4</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>8</v>
+      </c>
+      <c r="E43" t="s">
+        <v>8</v>
+      </c>
+      <c r="F43" t="s">
+        <v>13</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B44">
+        <v>4</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>8</v>
+      </c>
+      <c r="E44" t="s">
+        <v>8</v>
+      </c>
+      <c r="F44" t="s">
+        <v>13</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>8</v>
+      </c>
+      <c r="E45" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>6</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>24</v>
+      </c>
+      <c r="E46" t="s">
+        <v>17</v>
+      </c>
+      <c r="F46" t="s">
+        <v>27</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>24</v>
+      </c>
+      <c r="E47" t="s">
+        <v>17</v>
+      </c>
+      <c r="F47" t="s">
+        <v>27</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>24</v>
+      </c>
+      <c r="E48" t="s">
+        <v>17</v>
+      </c>
+      <c r="F48" t="s">
+        <v>27</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>24</v>
+      </c>
+      <c r="E49" t="s">
+        <v>17</v>
+      </c>
+      <c r="F49" t="s">
+        <v>27</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50">
+        <v>2</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>24</v>
+      </c>
+      <c r="E50" t="s">
+        <v>17</v>
+      </c>
+      <c r="F50" t="s">
+        <v>27</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>3</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>24</v>
+      </c>
+      <c r="E51" t="s">
+        <v>17</v>
+      </c>
+      <c r="F51" t="s">
+        <v>27</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>4</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>24</v>
+      </c>
+      <c r="E52" t="s">
+        <v>17</v>
+      </c>
+      <c r="F52" t="s">
+        <v>27</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B53">
+        <v>5</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>24</v>
+      </c>
+      <c r="E53" t="s">
+        <v>17</v>
+      </c>
+      <c r="F53" t="s">
+        <v>27</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B54">
+        <v>6</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>24</v>
+      </c>
+      <c r="E54" t="s">
+        <v>17</v>
+      </c>
+      <c r="F54" t="s">
+        <v>27</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H54" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>